<commit_message>
HD9 CFx Bom webpage
</commit_message>
<xml_diff>
--- a/bom/Option_HD9_CFx_MGN9.xlsx
+++ b/bom/Option_HD9_CFx_MGN9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03576FCF-ED31-49A5-8289-FF2DDB09360B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F225035-FBB3-429F-840B-ADECB1DDDE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -312,6 +312,12 @@
   </si>
   <si>
     <t>18a</t>
+  </si>
+  <si>
+    <t>HevORT/files/STL/HD9/Option_HD9_CFx at master · MirageC79/HevORT (github.com)</t>
+  </si>
+  <si>
+    <t>GitHub</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -544,23 +550,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="6" tint="-0.249977111117893"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="6" tint="-0.249977111117893"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -610,9 +605,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -625,32 +617,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -664,12 +641,50 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -683,23 +698,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -747,6 +745,20 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="6" tint="-0.249977111117893"/>
@@ -754,23 +766,6 @@
         <right style="thin">
           <color theme="6" tint="-0.249977111117893"/>
         </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-        <right/>
         <top style="thin">
           <color theme="6" tint="-0.249977111117893"/>
         </top>
@@ -835,7 +830,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="6" tint="-0.249977111117893"/>
@@ -894,42 +889,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1053,6 +1012,25 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color theme="6" tint="-0.249977111117893"/>
@@ -1067,16 +1045,15 @@
         <right style="thin">
           <color theme="6" tint="-0.249977111117893"/>
         </right>
-        <top style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="6" tint="-0.249977111117893"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="6" tint="-0.249977111117893"/>
+        </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2219,25 +2196,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C52D0CD-8C88-4E4D-9402-200FFB17A9F1}" name="Table1" displayName="Table1" ref="A1:L25" totalsRowShown="0" headerRowDxfId="3" dataDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9C52D0CD-8C88-4E4D-9402-200FFB17A9F1}" name="Table1" displayName="Table1" ref="A1:L25" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A1:L25" xr:uid="{9C52D0CD-8C88-4E4D-9402-200FFB17A9F1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L25">
     <sortCondition ref="B2:B25"/>
     <sortCondition ref="E2:E25"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A66386C4-C1F2-46F4-B3BF-C96CFA20F059}" name="SubAssy" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{E8CB70CF-BFCA-4B5A-8881-C383BA49617D}" name="Category" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{29E181D5-B628-4916-8428-1E94FC914B56}" name="Item" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{E10C1A08-7847-409F-BEB0-A4F0C690C948}" name="Thumbnail" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{2063F833-FC19-494C-AB3C-091DB1EB918F}" name="Part Name" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{8F190942-A290-4D02-93AF-E22E24328B55}" name="Part Description" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{5FE2C786-49C1-4789-8AFF-A49EF408914B}" name="Make/Buy" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{5ADFA761-04B8-47C9-B977-66D81358664A}" name="Included in _x000a_XYHD9_CFx kit?" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{B7D54B57-2235-4849-A86F-6BE437DD3179}" name="QTY" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{590B3964-DEF5-455A-9CD6-9A9021CFCF04}" name="Comment" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A66386C4-C1F2-46F4-B3BF-C96CFA20F059}" name="SubAssy" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{E8CB70CF-BFCA-4B5A-8881-C383BA49617D}" name="Category" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{29E181D5-B628-4916-8428-1E94FC914B56}" name="Item" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{E10C1A08-7847-409F-BEB0-A4F0C690C948}" name="Thumbnail" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{2063F833-FC19-494C-AB3C-091DB1EB918F}" name="Part Name" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{8F190942-A290-4D02-93AF-E22E24328B55}" name="Part Description" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{5FE2C786-49C1-4789-8AFF-A49EF408914B}" name="Make/Buy" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{5ADFA761-04B8-47C9-B977-66D81358664A}" name="Included in _x000a_XYHD9_CFx kit?" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{B7D54B57-2235-4849-A86F-6BE437DD3179}" name="QTY" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{590B3964-DEF5-455A-9CD6-9A9021CFCF04}" name="Comment" dataDxfId="2"/>
     <tableColumn id="11" xr3:uid="{086A86B1-C668-484B-8271-59E34F35AE57}" name="Vendor" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{5F6478B1-CCFF-4875-A723-D6E78D4B8A1E}" name="Vendor URL" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{5F6478B1-CCFF-4875-A723-D6E78D4B8A1E}" name="Vendor URL" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2566,7 +2543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2647,11 +2626,11 @@
       <c r="I2" s="13">
         <v>4</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="25" t="s">
         <v>79</v>
       </c>
       <c r="K2" s="16"/>
-      <c r="L2" s="17"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
@@ -2677,11 +2656,11 @@
       <c r="I3" s="13">
         <v>2</v>
       </c>
-      <c r="J3" s="32"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="17" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2709,11 +2688,11 @@
       <c r="I4" s="13">
         <v>2</v>
       </c>
-      <c r="J4" s="32"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="17" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2731,7 +2710,7 @@
       <c r="E5" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="22" t="s">
         <v>70</v>
       </c>
       <c r="G5" s="13"/>
@@ -2739,13 +2718,13 @@
       <c r="I5" s="13">
         <v>1</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="L5" s="17"/>
+      <c r="L5" s="29"/>
     </row>
     <row r="6" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
@@ -2771,13 +2750,13 @@
       <c r="I6" s="13">
         <v>1</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="26" t="s">
         <v>59</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="L6" s="17" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2805,11 +2784,11 @@
       <c r="I7" s="13">
         <v>1</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="26" t="s">
         <v>66</v>
       </c>
       <c r="K7" s="16"/>
-      <c r="L7" s="17"/>
+      <c r="L7" s="29"/>
     </row>
     <row r="8" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
@@ -2835,11 +2814,11 @@
       <c r="I8" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="26" t="s">
         <v>63</v>
       </c>
       <c r="K8" s="16"/>
-      <c r="L8" s="17"/>
+      <c r="L8" s="29"/>
     </row>
     <row r="9" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
@@ -2865,11 +2844,11 @@
       <c r="I9" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="26" t="s">
         <v>65</v>
       </c>
       <c r="K9" s="16"/>
-      <c r="L9" s="17"/>
+      <c r="L9" s="29"/>
     </row>
     <row r="10" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
@@ -2895,9 +2874,9 @@
       <c r="I10" s="13">
         <v>4</v>
       </c>
-      <c r="J10" s="32"/>
+      <c r="J10" s="26"/>
       <c r="K10" s="16"/>
-      <c r="L10" s="17"/>
+      <c r="L10" s="29"/>
     </row>
     <row r="11" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
@@ -2919,9 +2898,9 @@
       <c r="I11" s="13">
         <v>4</v>
       </c>
-      <c r="J11" s="32"/>
+      <c r="J11" s="26"/>
       <c r="K11" s="16"/>
-      <c r="L11" s="17"/>
+      <c r="L11" s="29"/>
     </row>
     <row r="12" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
@@ -2947,9 +2926,9 @@
       <c r="I12" s="13">
         <v>2</v>
       </c>
-      <c r="J12" s="32"/>
+      <c r="J12" s="26"/>
       <c r="K12" s="16"/>
-      <c r="L12" s="17"/>
+      <c r="L12" s="29"/>
     </row>
     <row r="13" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
@@ -2975,9 +2954,9 @@
       <c r="I13" s="13">
         <v>4</v>
       </c>
-      <c r="J13" s="32"/>
+      <c r="J13" s="26"/>
       <c r="K13" s="16"/>
-      <c r="L13" s="17"/>
+      <c r="L13" s="29"/>
     </row>
     <row r="14" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
@@ -3003,11 +2982,11 @@
       <c r="I14" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="26" t="s">
         <v>80</v>
       </c>
       <c r="K14" s="16"/>
-      <c r="L14" s="17"/>
+      <c r="L14" s="29"/>
     </row>
     <row r="15" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
@@ -3033,9 +3012,9 @@
       <c r="I15" s="13">
         <v>2</v>
       </c>
-      <c r="J15" s="32"/>
+      <c r="J15" s="26"/>
       <c r="K15" s="16"/>
-      <c r="L15" s="17"/>
+      <c r="L15" s="29"/>
     </row>
     <row r="16" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
@@ -3061,9 +3040,9 @@
       <c r="I16" s="13">
         <v>2</v>
       </c>
-      <c r="J16" s="32"/>
+      <c r="J16" s="26"/>
       <c r="K16" s="16"/>
-      <c r="L16" s="17"/>
+      <c r="L16" s="29"/>
     </row>
     <row r="17" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
@@ -3089,9 +3068,9 @@
       <c r="I17" s="13">
         <v>2</v>
       </c>
-      <c r="J17" s="32"/>
+      <c r="J17" s="26"/>
       <c r="K17" s="16"/>
-      <c r="L17" s="17"/>
+      <c r="L17" s="29"/>
     </row>
     <row r="18" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
@@ -3117,9 +3096,9 @@
       <c r="I18" s="13">
         <v>2</v>
       </c>
-      <c r="J18" s="32"/>
+      <c r="J18" s="26"/>
       <c r="K18" s="16"/>
-      <c r="L18" s="17"/>
+      <c r="L18" s="29"/>
     </row>
     <row r="19" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
@@ -3145,11 +3124,15 @@
       <c r="I19" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="J19" s="32" t="s">
+      <c r="J19" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="K19" s="16"/>
-      <c r="L19" s="17"/>
+      <c r="K19" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="30" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
@@ -3175,11 +3158,15 @@
       <c r="I20" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="J20" s="32" t="s">
+      <c r="J20" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="17"/>
+      <c r="K20" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L20" s="30" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="21" spans="1:12" customFormat="1" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
@@ -3188,24 +3175,28 @@
       <c r="B21" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="24">
         <v>19</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="25" t="s">
+      <c r="D21" s="23"/>
+      <c r="E21" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28" t="s">
+      <c r="F21" s="23"/>
+      <c r="G21" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="27"/>
-      <c r="I21" s="28">
+      <c r="H21" s="23"/>
+      <c r="I21" s="24">
         <v>2</v>
       </c>
-      <c r="J21" s="33"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="30"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L21" s="30" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
@@ -3214,7 +3205,7 @@
       <c r="B22" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="24">
         <v>20</v>
       </c>
       <c r="D22" s="14"/>
@@ -3231,9 +3222,13 @@
       <c r="I22" s="13">
         <v>1</v>
       </c>
-      <c r="J22" s="32"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="17"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" s="30" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
@@ -3242,7 +3237,7 @@
       <c r="B23" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="24">
         <v>21</v>
       </c>
       <c r="D23" s="14"/>
@@ -3259,9 +3254,13 @@
       <c r="I23" s="13">
         <v>1</v>
       </c>
-      <c r="J23" s="32"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="17"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L23" s="30" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
@@ -3270,7 +3269,7 @@
       <c r="B24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="24">
         <v>22</v>
       </c>
       <c r="D24" s="14"/>
@@ -3287,37 +3286,45 @@
       <c r="I24" s="13">
         <v>1</v>
       </c>
-      <c r="J24" s="32"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="17"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L24" s="30" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="28">
+      <c r="C25" s="24">
         <v>23</v>
       </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21" t="s">
+      <c r="D25" s="19"/>
+      <c r="E25" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G25" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19">
+      <c r="H25" s="18"/>
+      <c r="I25" s="18">
         <v>1</v>
       </c>
-      <c r="J25" s="34"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="23"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="L25" s="30" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
@@ -3326,11 +3333,16 @@
     <hyperlink ref="L4" r:id="rId2" xr:uid="{D72E9BE1-F02C-4023-BC69-9AD99242D3E9}"/>
     <hyperlink ref="K5" location="MGN9_Rail_Length!A1" display="Hiwin Specs" xr:uid="{AD8D94A3-017C-43A2-B6E2-29E4F540A98B}"/>
     <hyperlink ref="L6" r:id="rId3" xr:uid="{557F6417-84B1-4DCF-A703-1ECE9F56E24D}"/>
+    <hyperlink ref="L19" r:id="rId4" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/HD9/Option_HD9_CFx" xr:uid="{EE3D4A1C-BF74-451B-A269-A243F26B2091}"/>
+    <hyperlink ref="L20:L25" r:id="rId5" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/HD9/Option_HD9_CFx" xr:uid="{3FCD168F-0F95-46BE-B56A-2199BD97AF2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId6"/>
+  <webPublishItems count="1">
+    <webPublishItem id="4722" divId="Option_HD9_CFx_MGN9_4722" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\Option_HD9_CFx_MGN9.htm" autoRepublish="1"/>
+  </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>